<commit_message>
Add a new initial
</commit_message>
<xml_diff>
--- a/data/homeloanoutput.xlsx
+++ b/data/homeloanoutput.xlsx
@@ -3,9 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="HomeLoan" sheetId="1" r:id="rId1"/>
-    <sheet name="InsuranceImpact" sheetId="2" r:id="rId2"/>
-    <sheet name="MaintenanceImpact" sheetId="3" r:id="rId3"/>
+    <sheet name="InsuranceImpact" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -399,181 +397,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Year</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Principal (A)</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Interest (B)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Taxes, Home Insurance &amp; Maintenance (C)</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Total Payment (A+B+C)</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Balance</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Loan Paid to Date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2025</v>
-      </c>
-      <c r="B2" t="str">
-        <v>₹ 8,106</v>
-      </c>
-      <c r="C2" t="str">
-        <v>₹ 4,349</v>
-      </c>
-      <c r="D2" t="str">
-        <v>₹ 22,500</v>
-      </c>
-      <c r="E2" t="str">
-        <v>₹ 34,955</v>
-      </c>
-      <c r="F2" t="str">
-        <v>₹ 91,894</v>
-      </c>
-      <c r="G2" t="str">
-        <v>8.11%</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026</v>
-      </c>
-      <c r="B3" t="str">
-        <v>₹ 17,343</v>
-      </c>
-      <c r="C3" t="str">
-        <v>₹ 7,567</v>
-      </c>
-      <c r="D3" t="str">
-        <v>₹ 45,000</v>
-      </c>
-      <c r="E3" t="str">
-        <v>₹ 69,910</v>
-      </c>
-      <c r="F3" t="str">
-        <v>₹ 74,551</v>
-      </c>
-      <c r="G3" t="str">
-        <v>25.45%</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2027</v>
-      </c>
-      <c r="B4" t="str">
-        <v>₹ 18,970</v>
-      </c>
-      <c r="C4" t="str">
-        <v>₹ 5,940</v>
-      </c>
-      <c r="D4" t="str">
-        <v>₹ 45,000</v>
-      </c>
-      <c r="E4" t="str">
-        <v>₹ 69,910</v>
-      </c>
-      <c r="F4" t="str">
-        <v>₹ 55,581</v>
-      </c>
-      <c r="G4" t="str">
-        <v>44.42%</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2028</v>
-      </c>
-      <c r="B5" t="str">
-        <v>₹ 20,750</v>
-      </c>
-      <c r="C5" t="str">
-        <v>₹ 4,160</v>
-      </c>
-      <c r="D5" t="str">
-        <v>₹ 45,000</v>
-      </c>
-      <c r="E5" t="str">
-        <v>₹ 69,910</v>
-      </c>
-      <c r="F5" t="str">
-        <v>₹ 34,831</v>
-      </c>
-      <c r="G5" t="str">
-        <v>65.17%</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2029</v>
-      </c>
-      <c r="B6" t="str">
-        <v>₹ 22,696</v>
-      </c>
-      <c r="C6" t="str">
-        <v>₹ 2,214</v>
-      </c>
-      <c r="D6" t="str">
-        <v>₹ 45,000</v>
-      </c>
-      <c r="E6" t="str">
-        <v>₹ 69,910</v>
-      </c>
-      <c r="F6" t="str">
-        <v>₹ 12,134</v>
-      </c>
-      <c r="G6" t="str">
-        <v>87.87%</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2030</v>
-      </c>
-      <c r="B7" t="str">
-        <v>₹ 12,134</v>
-      </c>
-      <c r="C7" t="str">
-        <v>₹ 321</v>
-      </c>
-      <c r="D7" t="str">
-        <v>₹ 22,500</v>
-      </c>
-      <c r="E7" t="str">
-        <v>₹ 34,955</v>
-      </c>
-      <c r="F7" t="str">
-        <v>₹ 0</v>
-      </c>
-      <c r="G7" t="str">
-        <v>100%</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -613,10 +436,10 @@
         <v>₹ 76,960</v>
       </c>
       <c r="D2" t="str">
-        <v>₹ 18,000</v>
+        <v>₹ 0</v>
       </c>
       <c r="E2" t="str">
-        <v>₹ 5,64,832</v>
+        <v>₹ 5,46,832</v>
       </c>
       <c r="F2" t="str">
         <v>₹ 15,35,129</v>
@@ -636,10 +459,10 @@
         <v>₹ 92,062</v>
       </c>
       <c r="D3" t="str">
-        <v>₹ 36,000</v>
+        <v>₹ 0</v>
       </c>
       <c r="E3" t="str">
-        <v>₹ 11,29,664</v>
+        <v>₹ 10,93,664</v>
       </c>
       <c r="F3" t="str">
         <v>₹ 5,33,527</v>
@@ -659,10 +482,10 @@
         <v>₹ 13,305</v>
       </c>
       <c r="D4" t="str">
-        <v>₹ 18,000</v>
+        <v>₹ 0</v>
       </c>
       <c r="E4" t="str">
-        <v>₹ 5,64,832</v>
+        <v>₹ 5,46,832</v>
       </c>
       <c r="F4" t="str">
         <v>₹ 0</v>
@@ -676,156 +499,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Year</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Principal (A)</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Interest (B)</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Taxes, Home Insurance &amp; Maintenance (C)</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Total Payment (A+B+C)</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Balance</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Loan Paid to Date</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2025</v>
-      </c>
-      <c r="B2" t="str">
-        <v>₹ 2,32,963</v>
-      </c>
-      <c r="C2" t="str">
-        <v>₹ 96,775</v>
-      </c>
-      <c r="D2" t="str">
-        <v>₹ 9,300</v>
-      </c>
-      <c r="E2" t="str">
-        <v>₹ 3,39,038</v>
-      </c>
-      <c r="F2" t="str">
-        <v>₹ 19,67,037</v>
-      </c>
-      <c r="G2" t="str">
-        <v>10.59%</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026</v>
-      </c>
-      <c r="B3" t="str">
-        <v>₹ 4,99,209</v>
-      </c>
-      <c r="C3" t="str">
-        <v>₹ 1,60,266</v>
-      </c>
-      <c r="D3" t="str">
-        <v>₹ 18,600</v>
-      </c>
-      <c r="E3" t="str">
-        <v>₹ 6,78,075</v>
-      </c>
-      <c r="F3" t="str">
-        <v>₹ 14,67,828</v>
-      </c>
-      <c r="G3" t="str">
-        <v>33.28%</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2027</v>
-      </c>
-      <c r="B4" t="str">
-        <v>₹ 5,47,124</v>
-      </c>
-      <c r="C4" t="str">
-        <v>₹ 1,12,351</v>
-      </c>
-      <c r="D4" t="str">
-        <v>₹ 18,600</v>
-      </c>
-      <c r="E4" t="str">
-        <v>₹ 6,78,075</v>
-      </c>
-      <c r="F4" t="str">
-        <v>₹ 9,20,704</v>
-      </c>
-      <c r="G4" t="str">
-        <v>58.15%</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2028</v>
-      </c>
-      <c r="B5" t="str">
-        <v>₹ 5,99,637</v>
-      </c>
-      <c r="C5" t="str">
-        <v>₹ 59,838</v>
-      </c>
-      <c r="D5" t="str">
-        <v>₹ 18,600</v>
-      </c>
-      <c r="E5" t="str">
-        <v>₹ 6,78,075</v>
-      </c>
-      <c r="F5" t="str">
-        <v>₹ 3,21,067</v>
-      </c>
-      <c r="G5" t="str">
-        <v>85.41%</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2029</v>
-      </c>
-      <c r="B6" t="str">
-        <v>₹ 3,21,067</v>
-      </c>
-      <c r="C6" t="str">
-        <v>₹ 8,670</v>
-      </c>
-      <c r="D6" t="str">
-        <v>₹ 9,300</v>
-      </c>
-      <c r="E6" t="str">
-        <v>₹ 3,39,038</v>
-      </c>
-      <c r="F6" t="str">
-        <v>₹ 0</v>
-      </c>
-      <c r="G6" t="str">
-        <v>100%</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>